<commit_message>
fix:checking date if already exist0
</commit_message>
<xml_diff>
--- a/static/uploads/student3rdyear.xlsx
+++ b/static/uploads/student3rdyear.xlsx
@@ -472,7 +472,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>15/1/2021</t>
+          <t>14/1/2021</t>
         </is>
       </c>
     </row>
@@ -526,12 +526,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>66.66666666666667</t>
+          <t>33.333333333333336</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -546,7 +546,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -600,12 +600,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>66.66666666666667</t>
+          <t>33.333333333333336</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -620,7 +620,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -637,12 +637,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>66.66666666666667</t>
+          <t>33.333333333333336</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -657,7 +657,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -674,12 +674,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>66.66666666666667</t>
+          <t>33.333333333333336</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -694,7 +694,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -711,12 +711,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>33.333333333333336</t>
+          <t>66.66666666666667</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -731,7 +731,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>P</t>
         </is>
       </c>
     </row>
@@ -822,12 +822,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>66.66666666666667</t>
+          <t>33.333333333333336</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -842,7 +842,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -1007,12 +1007,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>66.66666666666667</t>
+          <t>33.333333333333336</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1027,7 +1027,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -1081,12 +1081,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>66.66666666666667</t>
+          <t>33.333333333333336</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -1192,12 +1192,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D21" s="2" t="inlineStr">
         <is>
-          <t>66.66666666666667</t>
+          <t>33.333333333333336</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1212,7 +1212,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -1340,12 +1340,12 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>66.66666666666667</t>
+          <t>33.333333333333336</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1360,7 +1360,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>A</t>
         </is>
       </c>
     </row>

</xml_diff>